<commit_message>
Calculo fecha de entrega y modificacion en tabla pedidos
</commit_message>
<xml_diff>
--- a/planning/assets/formatsXlsx/Pedidos.xlsx
+++ b/planning/assets/formatsXlsx/Pedidos.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25427"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6E9484A-4E56-49E3-B63C-DFA1AB5F7AE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="300" windowWidth="14880" windowHeight="7815"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -14,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>referencia_producto</t>
   </si>
@@ -31,17 +32,26 @@
     <t>cliente</t>
   </si>
   <si>
+    <t>cantidad_pendiente</t>
+  </si>
+  <si>
+    <t>fecha_minima</t>
+  </si>
+  <si>
+    <t>fecha_maxima</t>
+  </si>
+  <si>
+    <t>dia_entrega</t>
+  </si>
+  <si>
     <t>cantidad_original</t>
-  </si>
-  <si>
-    <t>cantidad_pendiente</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -68,6 +78,17 @@
       <name val="Comic Sans MS"/>
       <family val="4"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -93,7 +114,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -108,161 +129,223 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:G6" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <tableColumns count="7">
-    <tableColumn id="1" name="pedido" dataDxfId="6"/>
-    <tableColumn id="2" name="fecha_pedido" dataDxfId="5"/>
-    <tableColumn id="3" name="referencia_producto" dataDxfId="4"/>
-    <tableColumn id="4" name="producto" dataDxfId="3"/>
-    <tableColumn id="5" name="cliente" dataDxfId="2"/>
-    <tableColumn id="6" name="cantidad_original" dataDxfId="1"/>
-    <tableColumn id="7" name="cantidad_pendiente" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla1" displayName="Tabla1" ref="A1:J5" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="pedido" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="fecha_pedido" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="fecha_minima" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="fecha_maxima" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="referencia_producto" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="producto" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="cliente" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{647A05B6-5BD7-4805-94E6-A66FFA3E241A}" name="cantidad_original" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{EADC4394-90EA-467F-87BA-4F22F378A565}" name="cantidad_pendiente" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{56FC76C2-96BD-4EF6-B8EC-815DE704DFC1}" name="dia_entrega" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -311,7 +394,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -343,9 +426,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -377,6 +478,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -552,25 +671,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="A2" sqref="A2:J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" customWidth="1"/>
+    <col min="2" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29" customWidth="1"/>
     <col min="6" max="6" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="31" customWidth="1"/>
     <col min="8" max="8" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.42578125" customWidth="1"/>
-    <col min="10" max="10" width="16.5703125" customWidth="1"/>
+    <col min="9" max="9" width="33.85546875" customWidth="1"/>
+    <col min="10" max="10" width="19.7109375" customWidth="1"/>
     <col min="11" max="11" width="29" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16.42578125" customWidth="1"/>
     <col min="13" max="13" width="32.140625" customWidth="1"/>
@@ -580,7 +698,7 @@
     <col min="17" max="17" width="30.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
@@ -588,22 +706,31 @@
         <v>3</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="H1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="J1" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -611,8 +738,11 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -620,8 +750,11 @@
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -629,8 +762,11 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -638,60 +774,61 @@
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-    </row>
-    <row r="18" spans="4:5" ht="21">
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+    </row>
+    <row r="17" spans="4:5" ht="21" x14ac:dyDescent="0.4">
+      <c r="D17" s="2"/>
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" spans="4:5" ht="21" x14ac:dyDescent="0.4">
       <c r="D18" s="2"/>
       <c r="E18" s="3"/>
     </row>
-    <row r="19" spans="4:5" ht="21">
+    <row r="19" spans="4:5" ht="21" x14ac:dyDescent="0.4">
       <c r="D19" s="2"/>
       <c r="E19" s="3"/>
     </row>
-    <row r="20" spans="4:5" ht="21">
+    <row r="20" spans="4:5" ht="21" x14ac:dyDescent="0.4">
       <c r="D20" s="2"/>
       <c r="E20" s="3"/>
     </row>
-    <row r="21" spans="4:5" ht="21">
+    <row r="21" spans="4:5" ht="21" x14ac:dyDescent="0.4">
       <c r="D21" s="2"/>
       <c r="E21" s="3"/>
     </row>
-    <row r="22" spans="4:5" ht="21">
+    <row r="22" spans="4:5" ht="21" x14ac:dyDescent="0.4">
       <c r="D22" s="2"/>
       <c r="E22" s="3"/>
     </row>
-    <row r="23" spans="4:5" ht="21">
+    <row r="23" spans="4:5" ht="21" x14ac:dyDescent="0.4">
       <c r="D23" s="2"/>
       <c r="E23" s="3"/>
     </row>
-    <row r="24" spans="4:5" ht="21">
+    <row r="24" spans="4:5" ht="21" x14ac:dyDescent="0.4">
       <c r="D24" s="2"/>
       <c r="E24" s="3"/>
     </row>
-    <row r="25" spans="4:5" ht="21">
+    <row r="25" spans="4:5" ht="21" x14ac:dyDescent="0.4">
       <c r="D25" s="2"/>
       <c r="E25" s="3"/>
     </row>
-    <row r="26" spans="4:5" ht="21">
+    <row r="26" spans="4:5" ht="21" x14ac:dyDescent="0.4">
       <c r="D26" s="2"/>
       <c r="E26" s="3"/>
     </row>
-    <row r="27" spans="4:5" ht="21">
-      <c r="D27" s="2"/>
-      <c r="E27" s="3"/>
-    </row>
-    <row r="28" spans="4:5">
-      <c r="D28" s="1"/>
+    <row r="27" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D27" s="1"/>
     </row>
   </sheetData>
+  <dataConsolidate/>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J5" xr:uid="{64CB260C-E6FB-479A-A77F-F0D1081A54DF}">
+      <formula1>"Lunes,Martes,Miercoles,Jueves,Viernes,Sabado,Domingo"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
   <tableParts count="1">

</xml_diff>